<commit_message>
New Excel sheets provided by Tom (and minor bug fixes)
</commit_message>
<xml_diff>
--- a/src/data/Application.xlsx
+++ b/src/data/Application.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mgsJ6sAVowZm9Gfu+Ye6Rp7+Blztg=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mi+K6LJuJUOrftxqwvKacBDXNXO6g=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
   <si>
     <r>
       <rPr>
@@ -132,13 +132,7 @@
     <t>myProject</t>
   </si>
   <si>
-    <t>I-10</t>
-  </si>
-  <si>
-    <t>D-3;D-19;D-4</t>
-  </si>
-  <si>
-    <t>A-9</t>
+    <t>D-3</t>
   </si>
   <si>
     <t>desktop</t>
@@ -169,11 +163,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b/>
@@ -192,11 +186,6 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <sz val="11.0"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -212,17 +201,14 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -437,20 +423,21 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="2" max="3" width="10.75"/>
-    <col customWidth="1" min="4" max="4" width="13.38"/>
-    <col customWidth="1" min="5" max="5" width="35.0"/>
-    <col customWidth="1" min="6" max="6" width="13.38"/>
-    <col customWidth="1" min="7" max="7" width="24.88"/>
-    <col customWidth="1" min="8" max="9" width="13.25"/>
-    <col customWidth="1" min="10" max="10" width="8.88"/>
-    <col customWidth="1" min="11" max="11" width="12.88"/>
-    <col customWidth="1" min="12" max="12" width="12.75"/>
-    <col customWidth="1" min="13" max="13" width="18.75"/>
-    <col customWidth="1" min="14" max="14" width="14.75"/>
-    <col customWidth="1" min="15" max="26" width="7.63"/>
+    <col customWidth="1" min="1" max="1" width="14.43"/>
+    <col customWidth="1" min="2" max="3" width="12.29"/>
+    <col customWidth="1" min="4" max="4" width="15.29"/>
+    <col customWidth="1" min="5" max="5" width="22.43"/>
+    <col customWidth="1" min="6" max="6" width="15.29"/>
+    <col customWidth="1" min="7" max="7" width="14.43"/>
+    <col customWidth="1" min="8" max="9" width="15.14"/>
+    <col customWidth="1" min="10" max="10" width="10.14"/>
+    <col customWidth="1" min="11" max="11" width="19.0"/>
+    <col customWidth="1" min="12" max="12" width="17.86"/>
+    <col customWidth="1" min="13" max="13" width="12.0"/>
+    <col customWidth="1" min="14" max="14" width="16.86"/>
+    <col customWidth="1" min="15" max="26" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -602,32 +589,28 @@
       <c r="D4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3"/>
+      <c r="F4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="3"/>
+      <c r="H4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="I4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="N4" s="3"/>
     </row>
@@ -696,7 +679,7 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -716,7 +699,7 @@
         <v>8.0</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -732,36 +715,36 @@
       <c r="N9" s="3"/>
     </row>
     <row r="10" ht="14.25" customHeight="1">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
     </row>
     <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
     </row>
     <row r="12" ht="14.25" customHeight="1"/>
     <row r="13" ht="14.25" customHeight="1"/>

</xml_diff>